<commit_message>
my dream it is
</commit_message>
<xml_diff>
--- a/Excel.sheet.xlsx
+++ b/Excel.sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Komal-All\git directries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E7A155-1C39-4FB3-A505-DAFFA8D6AB68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8065B98-7B49-490F-8342-4B640817ED1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>kojoaduiodhakdhlahknk</t>
+    <t>komal sur</t>
   </si>
 </sst>
 </file>

</xml_diff>